<commit_message>
Test Script changes for ASC-Initial Version
</commit_message>
<xml_diff>
--- a/testdata/MasterData_ASC_UAT.xlsx
+++ b/testdata/MasterData_ASC_UAT.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="588" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="588" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="340" r:id="rId1"/>
-    <sheet name="scripts" sheetId="307" r:id="rId2"/>
-    <sheet name="opportunities" sheetId="341" r:id="rId3"/>
-    <sheet name="Quote_ProposalSetup" sheetId="342" r:id="rId4"/>
+    <sheet name="Deal_Analysis" sheetId="343" r:id="rId2"/>
+    <sheet name="scripts" sheetId="307" r:id="rId3"/>
+    <sheet name="opportunities" sheetId="341" r:id="rId4"/>
+    <sheet name="Quote_ProposalSetup" sheetId="342" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -27,54 +28,6 @@
     <author>Shantanu Shukla</author>
   </authors>
   <commentList>
-    <comment ref="H4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Shantanu Shukla:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Search for an Opportunity which has Quote available</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Shantanu Shukla:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Pass the Quote Number against Opportunity passed</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
@@ -123,12 +76,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="H6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shantanu Shukla:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Search for an Opportunity which has Quote available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shantanu Shukla:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Pass the Quote Number against Opportunity passed</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="93">
   <si>
     <t>Run</t>
   </si>
@@ -175,12 +176,6 @@
     <t>164716 - Account Setup</t>
   </si>
   <si>
-    <t>anshuman.sharma@stryker.com.uat</t>
-  </si>
-  <si>
-    <t>welcome12#</t>
-  </si>
-  <si>
     <t xml:space="preserve">164723 - This is to validate fields in the ASC Account Page Layout </t>
   </si>
   <si>
@@ -280,15 +275,6 @@
     <t>ASC pricing team user</t>
   </si>
   <si>
-    <t>armsales2@stryker.com.uat</t>
-  </si>
-  <si>
-    <t>ascfinance2@stryker.com.uat</t>
-  </si>
-  <si>
-    <t>ascpricingteam2@stryker.com.uat</t>
-  </si>
-  <si>
     <t>Spend_Type</t>
   </si>
   <si>
@@ -350,18 +336,111 @@
   </si>
   <si>
     <t>TestDescription</t>
+  </si>
+  <si>
+    <t>quote_ProposalSetup_227820_TC_03</t>
+  </si>
+  <si>
+    <t>Part_Number1</t>
+  </si>
+  <si>
+    <t>Part_Number2</t>
+  </si>
+  <si>
+    <t>Part_Number3</t>
+  </si>
+  <si>
+    <t>6506000000</t>
+  </si>
+  <si>
+    <t>1608-002-061</t>
+  </si>
+  <si>
+    <t>quote_ProposalSetup_184671_TC_013</t>
+  </si>
+  <si>
+    <t>quote_ProposalSetup_227904_TC_012</t>
+  </si>
+  <si>
+    <t>Capital</t>
+  </si>
+  <si>
+    <t>Emergency Care</t>
+  </si>
+  <si>
+    <t>Evacuation</t>
+  </si>
+  <si>
+    <t>Evacuation Chair and Accessories</t>
+  </si>
+  <si>
+    <t>Rebate_Percenatge</t>
+  </si>
+  <si>
+    <t>Rebate_Amount</t>
+  </si>
+  <si>
+    <t>249</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>quote_ProposalSetup_232246_TC_014</t>
+  </si>
+  <si>
+    <t>armsales2@stryker.com.uat2</t>
+  </si>
+  <si>
+    <t>stryker123</t>
+  </si>
+  <si>
+    <t>ascfinanceteam2@stryker.com.uat2</t>
+  </si>
+  <si>
+    <t>ascpricingteam2@stryker.com.uat2</t>
+  </si>
+  <si>
+    <t>shantanu.shukla@stryker.com.uat2</t>
+  </si>
+  <si>
+    <t>Acccount_Name</t>
+  </si>
+  <si>
+    <t>dealAnalysis_Finance_227824_TC_01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -509,48 +588,53 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -559,7 +643,21 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -988,13 +1086,13 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
@@ -1033,10 +1131,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>16</v>
+        <v>90</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="4"/>
@@ -1049,13 +1147,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>16</v>
+        <v>45</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1063,13 +1161,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>16</v>
+        <v>46</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1077,13 +1175,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>16</v>
+        <v>47</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1102,6 +1200,115 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" customWidth="1"/>
+    <col min="9" max="9" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="11">
+        <v>227824</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="11">
+        <v>227849</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -1138,10 +1345,10 @@
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1156,8 +1363,8 @@
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>18</v>
+      <c r="B3" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>14</v>
@@ -1169,18 +1376,18 @@
         <v>227835</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>17</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>8</v>
@@ -1189,18 +1396,18 @@
         <v>227836</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>17</v>
+      <c r="B5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>8</v>
@@ -1209,18 +1416,18 @@
         <v>227837</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>17</v>
+      <c r="B6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>8</v>
@@ -1229,18 +1436,18 @@
         <v>227838</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>17</v>
+      <c r="B7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>8</v>
@@ -1249,15 +1456,15 @@
         <v>227839</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>23</v>
+      <c r="B8" s="15" t="s">
+        <v>21</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>8</v>
@@ -1266,15 +1473,15 @@
         <v>227840</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>24</v>
+      <c r="B9" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>8</v>
@@ -1283,15 +1490,15 @@
         <v>227841</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>25</v>
+      <c r="B10" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>8</v>
@@ -1300,15 +1507,15 @@
         <v>227842</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>26</v>
+      <c r="B11" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>8</v>
@@ -1317,15 +1524,15 @@
         <v>227843</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>27</v>
+      <c r="B12" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>8</v>
@@ -1334,15 +1541,15 @@
         <v>227844</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>28</v>
+      <c r="B13" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>8</v>
@@ -1351,15 +1558,15 @@
         <v>227845</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>29</v>
+      <c r="B14" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>8</v>
@@ -1368,15 +1575,15 @@
         <v>227846</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>30</v>
+      <c r="B15" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>8</v>
@@ -1385,15 +1592,15 @@
         <v>227847</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>31</v>
+      <c r="B16" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>8</v>
@@ -1402,15 +1609,15 @@
         <v>227848</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>32</v>
+      <c r="B17" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>8</v>
@@ -1419,15 +1626,15 @@
         <v>227849</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>33</v>
+      <c r="B18" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>8</v>
@@ -1436,15 +1643,15 @@
         <v>227850</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>34</v>
+      <c r="B19" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>8</v>
@@ -1453,15 +1660,15 @@
         <v>227851</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>35</v>
+      <c r="B20" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>8</v>
@@ -1470,15 +1677,15 @@
         <v>227852</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>39</v>
+      <c r="B21" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>8</v>
@@ -1487,15 +1694,15 @@
         <v>227853</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>40</v>
+      <c r="B22" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>8</v>
@@ -1504,15 +1711,15 @@
         <v>227854</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>41</v>
+      <c r="B23" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>8</v>
@@ -1521,18 +1728,18 @@
         <v>227855</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>42</v>
+      <c r="B24" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>8</v>
@@ -1541,18 +1748,18 @@
         <v>227856</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>45</v>
+      <c r="B25" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>8</v>
@@ -1561,14 +1768,14 @@
         <v>227857</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="15"/>
       <c r="D26" s="10" t="s">
         <v>8</v>
       </c>
@@ -1576,14 +1783,14 @@
         <v>227858</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="15"/>
       <c r="D27" s="10" t="s">
         <v>8</v>
       </c>
@@ -1591,14 +1798,14 @@
         <v>227859</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="16"/>
+      <c r="B28" s="15"/>
       <c r="D28" s="10" t="s">
         <v>8</v>
       </c>
@@ -1606,14 +1813,14 @@
         <v>227860</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="16"/>
+      <c r="B29" s="15"/>
       <c r="D29" s="10" t="s">
         <v>8</v>
       </c>
@@ -1621,7 +1828,7 @@
         <v>227861</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1694,7 +1901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -1731,18 +1938,18 @@
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>31</v>
+      <c r="B2" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>8</v>
@@ -1751,15 +1958,15 @@
         <v>227848</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>32</v>
+      <c r="B3" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>8</v>
@@ -1768,15 +1975,15 @@
         <v>227849</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>33</v>
+      <c r="B4" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>8</v>
@@ -1785,15 +1992,15 @@
         <v>227850</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>34</v>
+      <c r="B5" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>8</v>
@@ -1802,15 +2009,15 @@
         <v>227851</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>35</v>
+      <c r="B6" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>8</v>
@@ -1819,15 +2026,15 @@
         <v>227852</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>39</v>
+      <c r="B7" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>8</v>
@@ -1836,15 +2043,15 @@
         <v>227853</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>40</v>
+      <c r="B8" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>8</v>
@@ -1853,15 +2060,15 @@
         <v>227854</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>41</v>
+      <c r="B9" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>8</v>
@@ -1870,18 +2077,18 @@
         <v>227855</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>42</v>
+      <c r="B10" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>8</v>
@@ -1890,18 +2097,18 @@
         <v>227856</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>45</v>
+      <c r="B11" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>8</v>
@@ -1910,14 +2117,14 @@
         <v>227857</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="15"/>
       <c r="D12" s="10" t="s">
         <v>8</v>
       </c>
@@ -1925,14 +2132,14 @@
         <v>227858</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="15"/>
       <c r="D13" s="10" t="s">
         <v>8</v>
       </c>
@@ -1940,14 +2147,14 @@
         <v>227859</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="15"/>
       <c r="D14" s="10" t="s">
         <v>8</v>
       </c>
@@ -1955,14 +2162,14 @@
         <v>227860</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="15"/>
       <c r="D15" s="10" t="s">
         <v>8</v>
       </c>
@@ -1970,7 +2177,7 @@
         <v>227861</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2003,18 +2210,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.5703125" style="1" collapsed="1"/>
-    <col min="2" max="2" width="33" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.140625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="37.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="22" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
@@ -2024,13 +2231,18 @@
     <col min="10" max="10" width="18.5703125" style="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="19.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="27.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="18.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16384" width="8.5703125" style="1" collapsed="1"/>
+    <col min="16" max="16" width="19.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="16384" width="8.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="30">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="30">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2047,42 +2259,57 @@
         <v>13</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="J1" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="O1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="S1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>46</v>
+      <c r="B2" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>8</v>
@@ -2091,30 +2318,30 @@
         <v>227848</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>59</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N2" s="19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>64</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>8</v>
@@ -2123,81 +2350,94 @@
         <v>227849</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="19">
+        <v>1588020122</v>
+      </c>
+      <c r="Q3" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="11">
+        <v>227820</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="11">
+        <v>227850</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="19">
+        <v>10000340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="11">
+        <v>227851</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="18" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="16" t="s">
+      <c r="I6" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="11">
-        <v>227850</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4" s="21">
-        <v>10000340</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="11">
-        <v>227851</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="D6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="11">
-        <v>227852</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="O6" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="15" t="s">
+        <v>76</v>
+      </c>
       <c r="D7" s="10" t="s">
         <v>8</v>
       </c>
@@ -2205,137 +2445,194 @@
         <v>227853</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <v>36</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="S7" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="T7" s="22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="D8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="11">
+        <v>227852</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="11">
         <v>227854</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="D9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="11">
+      <c r="F9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="11">
         <v>227855</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="D10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="11">
+      <c r="F10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="D11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="11">
         <v>227856</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="D11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="11">
+      <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="D12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="11">
         <v>227857</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="D12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="11">
+      <c r="F12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="D13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="11">
         <v>227858</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="D13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="11">
+      <c r="F13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="D14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11">
         <v>227859</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="D14" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="11">
+      <c r="F14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="D15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="11">
         <v>227860</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="D15" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="11">
+      <c r="F15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="D16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="11">
         <v>227861</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>38</v>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A7">
+  <conditionalFormatting sqref="A2:A8">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2343,7 +2640,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:A15">
+  <conditionalFormatting sqref="A9:A16">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2352,7 +2649,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A16">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
ASC Test Scripts updated
</commit_message>
<xml_diff>
--- a/testdata/MasterData_ASC_UAT.xlsx
+++ b/testdata/MasterData_ASC_UAT.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="94">
   <si>
     <t>Run</t>
   </si>
@@ -408,18 +408,28 @@
   </si>
   <si>
     <t>dealAnalysis_Finance_227824_TC_01</t>
+  </si>
+  <si>
+    <t>dealAnalysis_Finance_231310_TC_02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -588,53 +598,54 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1086,7 +1097,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1204,7 +1215,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1273,21 +1284,17 @@
         <v>9</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="11">
-        <v>227849</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>231310</v>
+      </c>
+      <c r="E3" s="25"/>
       <c r="F3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
   </sheetData>
@@ -1312,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -1775,7 +1782,9 @@
       <c r="A26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="15"/>
+      <c r="B26" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="D26" s="10" t="s">
         <v>8</v>
       </c>
@@ -1790,12 +1799,14 @@
       <c r="A27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="D27" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="11">
-        <v>227859</v>
+        <v>231310</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Added Test Scripts: dealAnalysis_Pricing_263023_TC_01, dealAnalysis_Pricing_263025_TC_03 for Deal Pricing Division
</commit_message>
<xml_diff>
--- a/testdata/MasterData_ASC_UAT.xlsx
+++ b/testdata/MasterData_ASC_UAT.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="108">
   <si>
     <t>Run</t>
   </si>
@@ -411,18 +411,88 @@
   </si>
   <si>
     <t>dealAnalysis_Finance_231310_TC_02</t>
+  </si>
+  <si>
+    <t>quote_ProposalSetup_262997_TC_01</t>
+  </si>
+  <si>
+    <t>!W1! - 164745 - Quote Page Layout - Sales RM</t>
+  </si>
+  <si>
+    <t>dealAnalysis_Pricing_263023_TC_01</t>
+  </si>
+  <si>
+    <t>Disposable_Part_Number</t>
+  </si>
+  <si>
+    <t>Capital_Part_Number</t>
+  </si>
+  <si>
+    <t>Service_Part_Number</t>
+  </si>
+  <si>
+    <t>0240200106</t>
+  </si>
+  <si>
+    <t>Test_Automation_Account_New</t>
+  </si>
+  <si>
+    <t>Test_Automation_Opportunity</t>
+  </si>
+  <si>
+    <t>dealAnalysis_Pricing_263025_TC_03</t>
+  </si>
+  <si>
+    <t>Test_Automation_Finance_Account</t>
+  </si>
+  <si>
+    <t>Test_Automation_Finance_Oppty</t>
+  </si>
+  <si>
+    <t>IDIN_Number</t>
+  </si>
+  <si>
+    <t>AMSURG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -572,7 +642,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -595,57 +665,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -654,7 +758,35 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1144,7 +1276,7 @@
       <c r="C2" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>87</v>
       </c>
       <c r="E2" s="5"/>
@@ -1154,46 +1286,61 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3">
+      <c r="A3" s="25">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>87</v>
       </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4">
+      <c r="A4" s="25">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>87</v>
       </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5">
+      <c r="A5" s="25">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>87</v>
       </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1212,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1225,12 +1372,16 @@
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="37" style="1" customWidth="1"/>
     <col min="8" max="8" width="34.140625" customWidth="1"/>
     <col min="9" max="9" width="28.140625" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
+    <row r="1" spans="1:13" ht="30">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1258,8 +1409,20 @@
       <c r="I1" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -1279,7 +1442,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:13">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1292,13 +1455,376 @@
       <c r="D3" s="11">
         <v>231310</v>
       </c>
-      <c r="E3" s="25"/>
+      <c r="E3" s="24"/>
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
+    <row r="4" spans="1:13" s="1" customFormat="1">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="11">
+        <v>263023</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" s="30">
+        <v>3910500322</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="29">
+        <v>77100003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="11">
+        <v>263025</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="30">
+        <v>3910500322</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" s="29">
+        <v>77100003</v>
+      </c>
+      <c r="M5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="9"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="9"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="9"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="9"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="9"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="9"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="9"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="9"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="9"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="9"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="9"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="9"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="9"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="9"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="9"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="9"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="9"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="9"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="9"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="9"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="9"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="9"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="9"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="9"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="9"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="9"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="9"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="9"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:A33">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1312,6 +1838,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2223,10 +2750,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I3"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -2343,7 +2870,7 @@
       <c r="M2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2366,24 +2893,24 @@
       <c r="H3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="19">
+      <c r="P3" s="18">
         <v>1588020122</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="Q3" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="R3" s="19" t="s">
+      <c r="R3" s="18" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="11">
@@ -2409,10 +2936,10 @@
       <c r="F5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="18">
         <v>10000340</v>
       </c>
     </row>
@@ -2432,10 +2959,10 @@
       <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="18" t="s">
         <v>66</v>
       </c>
       <c r="O6" s="1" t="s">
@@ -2470,13 +2997,13 @@
       <c r="M7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="N7" s="17" t="s">
+      <c r="N7" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="S7" s="23" t="s">
+      <c r="S7" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="T7" s="22" t="s">
+      <c r="T7" s="21" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2508,7 +3035,7 @@
       <c r="M8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N8" s="17" t="s">
+      <c r="N8" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2639,6 +3166,26 @@
         <v>227861</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="11">
+        <v>262997</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2651,7 +3198,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A16">
+  <conditionalFormatting sqref="A9:A17">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Test Scripts added for Deal Analysis- Pricing modules
</commit_message>
<xml_diff>
--- a/testdata/MasterData_ASC_UAT.xlsx
+++ b/testdata/MasterData_ASC_UAT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="588" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="588" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="340" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <author>Shantanu Shukla</author>
   </authors>
   <commentList>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
+    <comment ref="I6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0">
+    <comment ref="J6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="123">
   <si>
     <t>Run</t>
   </si>
@@ -453,18 +453,91 @@
   </si>
   <si>
     <t>AMSURG</t>
+  </si>
+  <si>
+    <t>Test_Automation_Pricing</t>
+  </si>
+  <si>
+    <t>Test_Pricing_Opportunity</t>
+  </si>
+  <si>
+    <t>dealAnalysis_Pricing_263024_TC_02</t>
+  </si>
+  <si>
+    <t>GPO_Pricelist</t>
+  </si>
+  <si>
+    <t>THE RESOURCE GROUP</t>
+  </si>
+  <si>
+    <t>dealAnalysis_Finance_263008_TC_01</t>
+  </si>
+  <si>
+    <t>dealAnalysis_Finance_263010_TC_02</t>
+  </si>
+  <si>
+    <t>quote_ProposalSetup_262999_TC_02</t>
+  </si>
+  <si>
+    <t>164752 - View Overall Deal Details</t>
+  </si>
+  <si>
+    <t>Account_Name</t>
+  </si>
+  <si>
+    <t>!W1! - 164735/164746/164748 - Opportunity/Quote Stages/Notifications (combine with quote stages) - SALES</t>
+  </si>
+  <si>
+    <t>quote_ProposalSetup_263002_TC_04</t>
+  </si>
+  <si>
+    <t>trinity_oppor762</t>
+  </si>
+  <si>
+    <t>quote_ProposalSetup_263003_TC_05</t>
+  </si>
+  <si>
+    <t>!W1! - 164735/164746/164748 - Opportunity/Quote Stages/Notifications (combine with quote stages) -FINANCE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -621,6 +694,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -679,59 +758,59 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -740,15 +819,28 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1229,7 +1321,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1359,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1370,7 +1462,7 @@
     <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" customWidth="1"/>
     <col min="7" max="7" width="37" style="1" customWidth="1"/>
     <col min="8" max="8" width="34.140625" customWidth="1"/>
@@ -1379,9 +1471,10 @@
     <col min="11" max="11" width="23.140625" customWidth="1"/>
     <col min="12" max="12" width="22.85546875" customWidth="1"/>
     <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30">
+    <row r="1" spans="1:14" ht="30">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1421,46 +1514,77 @@
       <c r="M1" s="34" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="11">
-        <v>227824</v>
+        <v>263008</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="J2" s="30">
+        <v>3910500322</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2" s="29">
+        <v>77100003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="11">
-        <v>231310</v>
+        <v>263010</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" s="1" customFormat="1">
+      <c r="J3" s="30">
+        <v>3910500322</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" s="29">
+        <v>77100003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -1492,28 +1616,25 @@
         <v>77100003</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="32" t="s">
+    <row r="5" spans="1:14" s="1" customFormat="1">
+      <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="11">
-        <v>263025</v>
-      </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="1"/>
+        <v>263024</v>
+      </c>
       <c r="G5" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I5" s="1"/>
+        <v>109</v>
+      </c>
       <c r="J5" s="30">
         <v>3910500322</v>
       </c>
@@ -1523,21 +1644,48 @@
       <c r="L5" s="29">
         <v>77100003</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="9"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="24"/>
+      <c r="N5" s="36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="11">
+        <v>263025</v>
+      </c>
       <c r="F6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="J6" s="30">
+        <v>3910500322</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L6" s="29">
+        <v>77100003</v>
+      </c>
+      <c r="M6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="9"/>
       <c r="B7" s="15"/>
       <c r="C7" s="10"/>
@@ -1547,7 +1695,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="9"/>
       <c r="B8" s="15"/>
       <c r="C8" s="10"/>
@@ -1557,7 +1705,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="9"/>
       <c r="B9" s="15"/>
       <c r="C9" s="10"/>
@@ -1567,7 +1715,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" s="9"/>
       <c r="B10" s="15"/>
       <c r="C10" s="10"/>
@@ -1577,7 +1725,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" s="9"/>
       <c r="B11" s="15"/>
       <c r="C11" s="10"/>
@@ -1587,7 +1735,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14">
       <c r="A12" s="9"/>
       <c r="B12" s="15"/>
       <c r="C12" s="10"/>
@@ -1597,7 +1745,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14">
       <c r="A13" s="9"/>
       <c r="B13" s="15"/>
       <c r="C13" s="10"/>
@@ -1607,7 +1755,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14">
       <c r="A14" s="9"/>
       <c r="B14" s="15"/>
       <c r="C14" s="10"/>
@@ -1617,7 +1765,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14">
       <c r="A15" s="9"/>
       <c r="B15" s="15"/>
       <c r="C15" s="10"/>
@@ -1627,7 +1775,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:14">
       <c r="A16" s="9"/>
       <c r="B16" s="15"/>
       <c r="C16" s="10"/>
@@ -1807,6 +1955,16 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="9"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
     <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
@@ -1816,7 +1974,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
+  <conditionalFormatting sqref="A4:A5">
     <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1824,7 +1982,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A33">
+  <conditionalFormatting sqref="A6:A34">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1838,7 +1996,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2750,37 +2908,40 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="1" collapsed="1"/>
-    <col min="2" max="2" width="36.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="99.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="20.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="33.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="19.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17" style="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="17.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="16384" width="8.5703125" style="1" collapsed="1"/>
+    <col min="6" max="6" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="30.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="19" width="14" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="23.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="21.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="16384" width="8.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="30">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="30">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2803,46 +2964,58 @@
         <v>35</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="V1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -2858,23 +3031,23 @@
       <c r="F2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="O2" s="16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:24">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2890,20 +3063,20 @@
       <c r="F3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="18">
+      <c r="Q3" s="18">
         <v>1588020122</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="R3" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="S3" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:24">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
@@ -2920,7 +3093,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:24">
       <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
@@ -2936,14 +3109,14 @@
       <c r="F5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="I5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="18">
+      <c r="J5" s="18">
         <v>10000340</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:24">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -2959,17 +3132,17 @@
       <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="I6" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="J6" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:24">
       <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
@@ -2985,29 +3158,29 @@
       <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="O7" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="S7" s="22" t="s">
+      <c r="T7" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="T7" s="21" t="s">
+      <c r="U7" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:24">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -3023,23 +3196,23 @@
       <c r="F8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N8" s="16" t="s">
+      <c r="O8" s="16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:24">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -3056,7 +3229,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:24">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -3076,7 +3249,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:24">
       <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
@@ -3094,7 +3267,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:24">
       <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
@@ -3109,7 +3282,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:24">
       <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
@@ -3124,7 +3297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:24">
       <c r="A14" s="9" t="s">
         <v>9</v>
       </c>
@@ -3139,7 +3312,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:24">
       <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
@@ -3154,7 +3327,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:24">
       <c r="A16" s="9" t="s">
         <v>9</v>
       </c>
@@ -3169,7 +3342,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:24">
       <c r="A17" s="26" t="s">
         <v>9</v>
       </c>
@@ -3187,6 +3360,108 @@
       </c>
       <c r="F17" s="1" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="11">
+        <v>262999</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V18" s="30">
+        <v>3910500322</v>
+      </c>
+      <c r="W18" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="X18" s="29">
+        <v>77100003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="11">
+        <v>263002</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="V19" s="30">
+        <v>3910500322</v>
+      </c>
+      <c r="W19" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="X19" s="29">
+        <v>77100003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="11">
+        <v>263003</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V20" s="30">
+        <v>3910500322</v>
+      </c>
+      <c r="W20" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="X20" s="29">
+        <v>77100003</v>
       </c>
     </row>
   </sheetData>
@@ -3198,7 +3473,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A17">
+  <conditionalFormatting sqref="A9:A20">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Test Script added for Quote Proposal
</commit_message>
<xml_diff>
--- a/testdata/MasterData_ASC_UAT.xlsx
+++ b/testdata/MasterData_ASC_UAT.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="127">
   <si>
     <t>Run</t>
   </si>
@@ -498,18 +498,37 @@
   </si>
   <si>
     <t>!W1! - 164735/164746/164748 - Opportunity/Quote Stages/Notifications (combine with quote stages) -FINANCE</t>
+  </si>
+  <si>
+    <t>quote_ProposalSetup_263004_TC_06</t>
+  </si>
+  <si>
+    <t>!W1! - 164735/164746/164748 - Opportunity/Quote Stages/Notifications (combine with quote stages) -PRICING</t>
+  </si>
+  <si>
+    <t>quote_ProposalSetup_263001_TC_03</t>
+  </si>
+  <si>
+    <t>164753 - Tier pricing calculations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -758,59 +777,59 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -819,25 +838,29 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -850,7 +873,21 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1454,7 +1491,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G5" sqref="G5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1967,26 +2004,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A5">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A34">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2529,58 +2566,58 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="21" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A29">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2878,18 +2915,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A7">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A15">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2908,10 +2945,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X20"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -3395,33 +3432,24 @@
       </c>
     </row>
     <row r="19" spans="1:24">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="42" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="43" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="11">
-        <v>263002</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>88</v>
+        <v>263001</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="V19" s="30">
         <v>3910500322</v>
       </c>
@@ -3433,26 +3461,32 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D20" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="38" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="11">
-        <v>263003</v>
+        <v>263002</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>105</v>
+        <v>120</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="V20" s="30">
         <v>3910500322</v>
@@ -3464,8 +3498,80 @@
         <v>77100003</v>
       </c>
     </row>
+    <row r="21" spans="1:24">
+      <c r="A21" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="11">
+        <v>263003</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V21" s="30">
+        <v>3910500322</v>
+      </c>
+      <c r="W21" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="X21" s="29">
+        <v>77100003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
+      <c r="A22" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="11">
+        <v>263004</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="V22" s="30">
+        <v>3910500322</v>
+      </c>
+      <c r="W22" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="X22" s="29">
+        <v>77100003</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A8">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:A21">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -3473,7 +3579,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A20">
+  <conditionalFormatting sqref="A22">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Test File Data Merged
</commit_message>
<xml_diff>
--- a/testdata/MasterData_ASC_UAT.xlsx
+++ b/testdata/MasterData_ASC_UAT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stryker-Repo\ASC-Automation\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayushv2\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="588" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="588" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="340" r:id="rId1"/>
@@ -177,7 +177,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="171">
   <si>
     <t>Run</t>
   </si>
@@ -467,9 +467,6 @@
     <t>!W1! - 164745 - Quote Page Layout - Sales RM</t>
   </si>
   <si>
-    <t>dealAnalysis_Pricing_263023_TC_01</t>
-  </si>
-  <si>
     <t>Disposable_Part_Number</t>
   </si>
   <si>
@@ -485,12 +482,6 @@
     <t>Test_Automation_Account_New</t>
   </si>
   <si>
-    <t>Test_Automation_Opportunity</t>
-  </si>
-  <si>
-    <t>dealAnalysis_Pricing_263025_TC_03</t>
-  </si>
-  <si>
     <t>Test_Automation_Finance_Account</t>
   </si>
   <si>
@@ -500,24 +491,12 @@
     <t>IDIN_Number</t>
   </si>
   <si>
-    <t>AMSURG</t>
-  </si>
-  <si>
     <t>Test_Automation_Pricing</t>
   </si>
   <si>
     <t>Test_Pricing_Opportunity</t>
   </si>
   <si>
-    <t>dealAnalysis_Pricing_263024_TC_02</t>
-  </si>
-  <si>
-    <t>GPO_Pricelist</t>
-  </si>
-  <si>
-    <t>THE RESOURCE GROUP</t>
-  </si>
-  <si>
     <t>dealAnalysis_Finance_263008_TC_01</t>
   </si>
   <si>
@@ -609,25 +588,123 @@
   </si>
   <si>
     <t>GEMINI ASC</t>
+  </si>
+  <si>
+    <t>Capital_Part_Number_2</t>
+  </si>
+  <si>
+    <t>Base_Price</t>
+  </si>
+  <si>
+    <t>Rebate_$</t>
+  </si>
+  <si>
+    <t>Net_Price_After_Rebate</t>
+  </si>
+  <si>
+    <t>Gross_margin_$</t>
+  </si>
+  <si>
+    <t>Gross_margin_%</t>
+  </si>
+  <si>
+    <t>Year1_qty</t>
+  </si>
+  <si>
+    <t>Year_1_PP</t>
+  </si>
+  <si>
+    <t>Year_1_BP</t>
+  </si>
+  <si>
+    <t>Year_1_NASP</t>
+  </si>
+  <si>
+    <t>Year_1_EC</t>
+  </si>
+  <si>
+    <t>Year_1_EPG</t>
+  </si>
+  <si>
+    <t>Cost_of_service</t>
+  </si>
+  <si>
+    <t>Unit_cost_applied</t>
+  </si>
+  <si>
+    <t>Capital_BU_Total</t>
+  </si>
+  <si>
+    <t>3910500322</t>
+  </si>
+  <si>
+    <t>dealAnalysis_Finance_263011_TC_03</t>
+  </si>
+  <si>
+    <t>0702-014-000</t>
+  </si>
+  <si>
+    <t>$157,998.06</t>
+  </si>
+  <si>
+    <t>$158,360.81</t>
+  </si>
+  <si>
+    <t>$107,273.70</t>
+  </si>
+  <si>
+    <t>$4,956,487.20</t>
+  </si>
+  <si>
+    <t>dealAnalysis_Finance_263012_TC_04</t>
+  </si>
+  <si>
+    <t>50,724.36</t>
+  </si>
+  <si>
+    <t>157,998.06</t>
+  </si>
+  <si>
+    <t>158,630.91</t>
+  </si>
+  <si>
+    <t>107,273.7</t>
+  </si>
+  <si>
+    <t>dealAnalysis_Finance_263013_TC_05</t>
+  </si>
+  <si>
+    <t>34,924.55</t>
+  </si>
+  <si>
+    <t>142,198.25</t>
+  </si>
+  <si>
+    <t>dealAnalysis_Finance_263014_TC_06</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>$10.00</t>
+  </si>
+  <si>
+    <t>Version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="36">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -849,12 +926,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF202124"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
@@ -924,58 +995,55 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -988,61 +1056,97 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="40" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1051,7 +1155,63 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1616,8 +1776,8 @@
       <c r="C3" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="56" t="s">
-        <v>138</v>
+      <c r="D3" s="50" t="s">
+        <v>131</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
@@ -1635,8 +1795,8 @@
       <c r="C4" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="56" t="s">
-        <v>138</v>
+      <c r="D4" s="50" t="s">
+        <v>131</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
@@ -1680,17 +1840,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" customWidth="1"/>
     <col min="7" max="7" width="37" style="1" customWidth="1"/>
@@ -1699,232 +1860,466 @@
     <col min="10" max="10" width="25" customWidth="1"/>
     <col min="11" max="11" width="23.140625" customWidth="1"/>
     <col min="12" max="12" width="22.85546875" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
     <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" customWidth="1"/>
+    <col min="18" max="19" width="16" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" customWidth="1"/>
+    <col min="24" max="25" width="12.140625" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:28" ht="30">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="N1" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="P1" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q1" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="R1" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="S1" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="T1" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="U1" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="V1" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="W1" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="X1" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y1" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z1" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA1" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB1" s="58" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="52">
+        <v>263008</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="52"/>
+      <c r="J2" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="M1" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="N1" s="34" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="11">
-        <v>263008</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="30">
-        <v>3910500322</v>
-      </c>
-      <c r="K2" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="L2" s="29">
+      <c r="L2" s="52">
         <v>77100003</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="11">
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="52"/>
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="52"/>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="52">
         <v>263010</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="30">
-        <v>3910500322</v>
-      </c>
-      <c r="K3" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="L3" s="29">
+      <c r="E3" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="52"/>
+      <c r="J3" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" s="52">
         <v>77100003</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="11">
-        <v>263023</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="61"/>
+      <c r="T3" s="61"/>
+      <c r="U3" s="61"/>
+      <c r="V3" s="61"/>
+      <c r="W3" s="61"/>
+      <c r="X3" s="61"/>
+      <c r="Y3" s="61"/>
+      <c r="Z3" s="52"/>
+      <c r="AA3" s="52"/>
+      <c r="AB3" s="52"/>
+    </row>
+    <row r="4" spans="1:28" s="1" customFormat="1">
+      <c r="A4" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="52">
+        <v>263011</v>
+      </c>
+      <c r="E4" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="J4" s="30">
-        <v>3910500322</v>
-      </c>
-      <c r="K4" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="L4" s="29">
+      <c r="I4" s="52"/>
+      <c r="J4" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="K4" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="52">
         <v>77100003</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" s="1" customFormat="1">
-      <c r="A5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="11">
-        <v>263024</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="J5" s="30">
-        <v>3910500322</v>
-      </c>
-      <c r="K5" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="L5" s="29">
+      <c r="M4" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="52">
+        <v>402</v>
+      </c>
+      <c r="U4" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="V4" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="W4" s="55" t="s">
+        <v>156</v>
+      </c>
+      <c r="X4" s="55" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="52"/>
+      <c r="AA4" s="52"/>
+      <c r="AB4" s="55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" s="1" customFormat="1">
+      <c r="A5" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="52">
+        <v>263012</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="52"/>
+      <c r="J5" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="K5" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="L5" s="52">
         <v>77100003</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="N5" s="36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="11">
-        <v>263025</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="30">
-        <v>3910500322</v>
-      </c>
-      <c r="K6" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="L6" s="29">
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="53">
+        <v>393.03</v>
+      </c>
+      <c r="P5" s="53">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="53">
+        <v>393.03</v>
+      </c>
+      <c r="R5" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="S5" s="52">
+        <v>32.1</v>
+      </c>
+      <c r="T5" s="52"/>
+      <c r="U5" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="V5" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="W5" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="X5" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y5" s="53">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="52"/>
+      <c r="AA5" s="52"/>
+      <c r="AB5" s="52"/>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="A6" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="52">
+        <v>263013</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="52"/>
+      <c r="J6" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="K6" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="52">
         <v>77100003</v>
       </c>
-      <c r="M6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="9"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52">
+        <v>353.73</v>
+      </c>
+      <c r="P6" s="53">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="52">
+        <v>353.73</v>
+      </c>
+      <c r="R6" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="S6" s="52">
+        <v>24.56</v>
+      </c>
+      <c r="T6" s="52"/>
+      <c r="U6" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="V6" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="W6" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="X6" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y6" s="53">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="52"/>
+      <c r="AA6" s="52"/>
+      <c r="AB6" s="52"/>
+    </row>
+    <row r="7" spans="1:28">
+      <c r="A7" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="52">
+        <v>263014</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="52"/>
+      <c r="J7" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="K7" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="L7" s="52">
+        <v>77100003</v>
+      </c>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="54"/>
+      <c r="S7" s="52"/>
+      <c r="T7" s="52"/>
+      <c r="U7" s="55"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="54"/>
+      <c r="Y7" s="53"/>
+      <c r="Z7" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA7" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB7" s="52"/>
+    </row>
+    <row r="8" spans="1:28">
       <c r="A8" s="9"/>
       <c r="B8" s="15"/>
       <c r="C8" s="10"/>
@@ -1934,7 +2329,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:28">
       <c r="A9" s="9"/>
       <c r="B9" s="15"/>
       <c r="C9" s="10"/>
@@ -1944,7 +2339,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:28">
       <c r="A10" s="9"/>
       <c r="B10" s="15"/>
       <c r="C10" s="10"/>
@@ -1954,7 +2349,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:28">
       <c r="A11" s="9"/>
       <c r="B11" s="15"/>
       <c r="C11" s="10"/>
@@ -1964,7 +2359,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:28">
       <c r="A12" s="9"/>
       <c r="B12" s="15"/>
       <c r="C12" s="10"/>
@@ -1974,7 +2369,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:28">
       <c r="A13" s="9"/>
       <c r="B13" s="15"/>
       <c r="C13" s="10"/>
@@ -1984,7 +2379,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:28">
       <c r="A14" s="9"/>
       <c r="B14" s="15"/>
       <c r="C14" s="10"/>
@@ -1994,7 +2389,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:28">
       <c r="A15" s="9"/>
       <c r="B15" s="15"/>
       <c r="C15" s="10"/>
@@ -2004,7 +2399,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:28">
       <c r="A16" s="9"/>
       <c r="B16" s="15"/>
       <c r="C16" s="10"/>
@@ -2195,37 +2590,64 @@
       <c r="I34" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+  <conditionalFormatting sqref="A8:A34">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="12" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A5">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:A34">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+  <conditionalFormatting sqref="A5">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A7">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K0000FFClassification: Internal&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2693,13 +3115,13 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="39" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="11">
@@ -2775,58 +3197,58 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A30">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2848,7 +3270,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -2870,426 +3292,426 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="46" t="s">
+      <c r="H1" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="40" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="49"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="49">
+      <c r="E2" s="43">
         <v>227848</v>
       </c>
-      <c r="F2" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
+      <c r="F2" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="48" t="s">
+      <c r="A3" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="49"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="49">
+      <c r="E3" s="43">
         <v>227849</v>
       </c>
-      <c r="F3" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
+      <c r="F3" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="48" t="s">
+      <c r="A4" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="49"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="43">
         <v>227850</v>
       </c>
-      <c r="F4" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
+      <c r="F4" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="48" t="s">
+      <c r="A5" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="49"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E5" s="43">
         <v>227851</v>
       </c>
-      <c r="F5" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
+      <c r="F5" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="48" t="s">
+      <c r="A6" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="49"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="49">
+      <c r="E6" s="43">
         <v>227852</v>
       </c>
-      <c r="F6" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
+      <c r="F6" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="48" t="s">
+      <c r="A7" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="49"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="43">
         <v>227853</v>
       </c>
-      <c r="F7" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
+      <c r="F7" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="48" t="s">
+      <c r="A8" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="49"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="49">
+      <c r="E8" s="43">
         <v>227854</v>
       </c>
-      <c r="F8" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
+      <c r="F8" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="48" t="s">
+      <c r="A9" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="49"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="43">
         <v>227855</v>
       </c>
-      <c r="F9" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="49" t="s">
+      <c r="F9" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="48" t="s">
+      <c r="A10" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="49"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="43">
         <v>227856</v>
       </c>
-      <c r="F10" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="49" t="s">
+      <c r="F10" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="49"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="48" t="s">
+      <c r="A11" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="49"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="43">
         <v>227857</v>
       </c>
-      <c r="F11" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
+      <c r="F11" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="49"/>
+      <c r="A12" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="43"/>
       <c r="D12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="49">
+      <c r="E12" s="43">
         <v>262996</v>
       </c>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="I12" s="51" t="s">
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="K12" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="L12" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="M12" s="50" t="s">
+      <c r="J12" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="K12" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="M12" s="44" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="49"/>
+      <c r="A13" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="43"/>
       <c r="D13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="49">
+      <c r="E13" s="43">
         <v>263383</v>
       </c>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
       <c r="H13" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I13" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="J13" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="K13" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="L13" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="M13" s="50" t="s">
+      <c r="J13" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="K13" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="L13" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="M13" s="44" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
+      <c r="A14" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="49">
+      <c r="E14" s="43">
         <v>227860</v>
       </c>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="49"/>
+      <c r="A15" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="42"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="49">
+      <c r="E15" s="43">
         <v>227861</v>
       </c>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A7">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A15">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3308,10 +3730,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -3339,10 +3761,12 @@
     <col min="23" max="23" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="21.5703125" style="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="35.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="16384" width="8.5703125" style="1" collapsed="1"/>
+    <col min="26" max="26" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="8.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" ht="30">
+    <row r="1" spans="1:27" s="2" customFormat="1" ht="30">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3365,7 +3789,7 @@
         <v>35</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>58</v>
@@ -3407,19 +3831,25 @@
         <v>82</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="X1" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="Y1" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
+        <v>126</v>
+      </c>
+      <c r="Z1" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA1" s="63" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -3451,7 +3881,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:27">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -3480,7 +3910,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:27">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
@@ -3497,7 +3927,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:27">
       <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
@@ -3520,7 +3950,7 @@
         <v>10000340</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:27">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -3546,7 +3976,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:27">
       <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
@@ -3584,7 +4014,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:27">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -3616,7 +4046,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:27">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -3633,7 +4063,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:27">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -3653,7 +4083,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:27">
       <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
@@ -3671,7 +4101,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:27">
       <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
@@ -3686,7 +4116,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:27">
       <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
@@ -3701,7 +4131,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:27">
       <c r="A14" s="9" t="s">
         <v>9</v>
       </c>
@@ -3716,7 +4146,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:27">
       <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
@@ -3731,7 +4161,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:27">
       <c r="A16" s="9" t="s">
         <v>9</v>
       </c>
@@ -3746,7 +4176,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:27">
       <c r="A17" s="26" t="s">
         <v>9</v>
       </c>
@@ -3766,78 +4196,78 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
-      <c r="A18" s="37" t="s">
+    <row r="18" spans="1:27">
+      <c r="A18" s="31" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D18" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="32" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="11">
         <v>262999</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="V18" s="30">
+        <v>102</v>
+      </c>
+      <c r="V18" s="29">
         <v>3910500322</v>
       </c>
-      <c r="W18" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="X18" s="29">
+      <c r="W18" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="X18" s="28">
         <v>77100003</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
-      <c r="A19" s="42" t="s">
+    <row r="19" spans="1:27">
+      <c r="A19" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="37" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="11">
         <v>263001</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="V19" s="30">
+        <v>101</v>
+      </c>
+      <c r="V19" s="29">
         <v>3910500322</v>
       </c>
-      <c r="W19" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="X19" s="29">
+      <c r="W19" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="X19" s="28">
         <v>77100003</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
-      <c r="A20" s="39" t="s">
+    <row r="20" spans="1:27">
+      <c r="A20" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D20" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="32" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="11">
@@ -3847,186 +4277,232 @@
         <v>88</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="V20" s="30">
+      <c r="V20" s="29">
         <v>3910500322</v>
       </c>
-      <c r="W20" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="X20" s="29">
+      <c r="W20" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="X20" s="28">
         <v>77100003</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
-      <c r="A21" s="40" t="s">
+    <row r="21" spans="1:27">
+      <c r="A21" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D21" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="35" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="11">
         <v>263003</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="V21" s="30">
+        <v>102</v>
+      </c>
+      <c r="V21" s="29">
         <v>3910500322</v>
       </c>
-      <c r="W21" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="X21" s="29">
+      <c r="W21" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="X21" s="28">
         <v>77100003</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
-      <c r="A22" s="40" t="s">
+    <row r="22" spans="1:27">
+      <c r="A22" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="35" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="11">
         <v>263004</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="V22" s="30">
+        <v>105</v>
+      </c>
+      <c r="V22" s="29">
         <v>3910500322</v>
       </c>
-      <c r="W22" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="X22" s="29">
+      <c r="W22" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="X22" s="28">
         <v>77100003</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
-      <c r="A23" s="52" t="s">
+    <row r="23" spans="1:27">
+      <c r="A23" s="46" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D23" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="47" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="11">
         <v>263028</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="V23" s="30">
+        <v>101</v>
+      </c>
+      <c r="V23" s="29">
         <v>3910500322</v>
       </c>
-      <c r="W23" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="X23" s="29">
+      <c r="W23" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="X23" s="28">
         <v>77100003</v>
       </c>
-      <c r="Y23" s="29" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25">
-      <c r="A24" s="54" t="s">
+      <c r="Y23" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27">
+      <c r="A24" s="48" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D24" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="49" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="11">
         <v>263029</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="V24" s="30">
+        <v>101</v>
+      </c>
+      <c r="V24" s="29">
         <v>3910500322</v>
       </c>
-      <c r="W24" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="X24" s="29">
+      <c r="W24" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="X24" s="28">
         <v>77100003</v>
       </c>
-      <c r="Y24" s="29" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25">
-      <c r="A25" s="54" t="s">
+      <c r="Y24" s="28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27">
+      <c r="A25" s="48" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="49" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="11">
         <v>263436</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="J25" s="18">
         <v>10000746</v>
       </c>
-      <c r="V25" s="30"/>
-      <c r="W25" s="31"/>
-      <c r="X25" s="29"/>
-      <c r="Y25" s="29" t="s">
-        <v>141</v>
+      <c r="V25" s="29"/>
+      <c r="W25" s="30"/>
+      <c r="X25" s="28"/>
+      <c r="Y25" s="28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27">
+      <c r="A26" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="11">
+        <v>263001</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="V26" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="W26" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="X26" s="28">
+        <v>77100003</v>
+      </c>
+      <c r="Z26" s="67">
+        <v>10367040</v>
+      </c>
+      <c r="AA26" s="28">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A8">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:A21 A23:A24">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -4034,7 +4510,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A21 A23:A24">
+  <conditionalFormatting sqref="A22">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -4042,7 +4518,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
+  <conditionalFormatting sqref="A25">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -4050,7 +4526,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
+  <conditionalFormatting sqref="A26">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -4059,7 +4535,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A16 A26">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>